<commit_message>
Tune (relative) paths and messages definition to use this project like as library.
</commit_message>
<xml_diff>
--- a/meta/messages/ja/MessagesJa.xlsx
+++ b/meta/messages/ja/MessagesJa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/messages/ja/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6F117D-9529-5149-8321-21306F8E2118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE06A72-6E48-2342-AE6C-C5F1B03243A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3280" yWindow="1740" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,10 +365,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>MessageesJa</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>messages</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -378,6 +374,10 @@
   </si>
   <si>
     <t>import {LocaleLabels} from "@/i18n/LocaleLabels"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>MessagesJa</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1659,8 +1659,8 @@
   </sheetPr>
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="36"/>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="36"/>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="93" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="94"/>
       <c r="E11" s="94"/>
@@ -1820,7 +1820,7 @@
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="93" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="94"/>
       <c r="E12" s="94"/>
@@ -2319,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41" s="41"/>
       <c r="D41" s="41"/>

</xml_diff>